<commit_message>
feat: v0.0.15 + v2.2.9 bear
</commit_message>
<xml_diff>
--- a/docs/03_strategies/DCA_Conditional_Buy_LR_with_TrailingStop/Bear/Binance_BTC-USDT_1d/equity_curve.xlsx
+++ b/docs/03_strategies/DCA_Conditional_Buy_LR_with_TrailingStop/Bear/Binance_BTC-USDT_1d/equity_curve.xlsx
@@ -400,7 +400,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -408,7 +408,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -416,7 +416,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -424,7 +424,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -432,7 +432,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -440,7 +440,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -448,7 +448,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -456,7 +456,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -472,7 +472,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -544,7 +544,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -576,7 +576,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -608,7 +608,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -720,7 +720,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -736,7 +736,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -776,31 +776,31 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>1598.82718468666</v>
+        <v>998.82718468666</v>
       </c>
       <c r="B49">
-        <v>0.0007330095708374396</v>
+        <v>0.001172815313340014</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>1599.51029929666</v>
+        <v>999.51029929666</v>
       </c>
       <c r="B50">
-        <v>0.0003060629395875702</v>
+        <v>0.0004897007033399792</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>1598.56929775666</v>
+        <v>998.56929775666</v>
       </c>
       <c r="B51">
-        <v>0.0008941889020874783</v>
+        <v>0.001430702243339965</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>1600.13675227666</v>
+        <v>1000.13675227666</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -811,295 +811,295 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>1599.68238700666</v>
+        <v>999.68238700666</v>
       </c>
       <c r="B53">
-        <v>0.0002839540241503791</v>
+        <v>0.0004543031430109812</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>1598.80786372666</v>
+        <v>998.80786372666</v>
       </c>
       <c r="B54">
-        <v>0.000830484362108086</v>
+        <v>0.001328706846313699</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>1598.16859603666</v>
+        <v>998.16859603666</v>
       </c>
       <c r="B55">
-        <v>0.001229992522326473</v>
+        <v>0.00196788712695517</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>1595.69009995666</v>
+        <v>995.69009995666</v>
       </c>
       <c r="B56">
-        <v>0.002778920185211198</v>
+        <v>0.004446044313318076</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>1595.30615833666</v>
+        <v>995.30615833666</v>
       </c>
       <c r="B57">
-        <v>0.003018863189741205</v>
+        <v>0.004829933435606559</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>1593.72817930666</v>
+        <v>993.72817930666</v>
       </c>
       <c r="B58">
-        <v>0.004005015796857303</v>
+        <v>0.006407696702887766</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>1593.84608296666</v>
+        <v>993.84608296666</v>
       </c>
       <c r="B59">
-        <v>0.003931332307097857</v>
+        <v>0.006289809164277016</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>1594.03854304666</v>
+        <v>994.03854304666</v>
       </c>
       <c r="B60">
-        <v>0.003811055037217015</v>
+        <v>0.006097375400032301</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>1593.99468571666</v>
+        <v>993.99468571666</v>
       </c>
       <c r="B61">
-        <v>0.003838463525858815</v>
+        <v>0.006141226733262783</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>1594.93866451666</v>
+        <v>994.93866451666</v>
       </c>
       <c r="B62">
-        <v>0.003248527197818651</v>
+        <v>0.005197377006861625</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>1596.16014268666</v>
+        <v>996.16014268666</v>
       </c>
       <c r="B63">
-        <v>0.002485168585961262</v>
+        <v>0.003976065853942279</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>1594.76254813666</v>
+        <v>994.76254813666</v>
       </c>
       <c r="B64">
-        <v>0.003358590528186878</v>
+        <v>0.005373469305838818</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>1595.28289198666</v>
+        <v>995.28289198666</v>
       </c>
       <c r="B65">
-        <v>0.003033403415735547</v>
+        <v>0.004853196604315269</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>1595.30821951666</v>
+        <v>995.30821951666</v>
       </c>
       <c r="B66">
-        <v>0.003017575062337574</v>
+        <v>0.004827872537439104</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>1595.29507168666</v>
+        <v>995.29507168666</v>
       </c>
       <c r="B67">
-        <v>0.003025791753805573</v>
+        <v>0.004841018569689215</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>1594.38936004666</v>
+        <v>994.38936004666</v>
       </c>
       <c r="B68">
-        <v>0.003591813150858991</v>
+        <v>0.005746606368495999</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69">
-        <v>1594.54603054666</v>
+        <v>994.5460305466599</v>
       </c>
       <c r="B69">
-        <v>0.003493902456802922</v>
+        <v>0.005589957290614067</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>1592.9676922805</v>
+        <v>992.9676922805</v>
       </c>
       <c r="B70">
-        <v>0.004480279567330769</v>
+        <v>0.007168079744935496</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>1590.8048603805</v>
+        <v>990.8048603805</v>
       </c>
       <c r="B71">
-        <v>0.005831933978694415</v>
+        <v>0.009330615913191176</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>1581.4484199805</v>
+        <v>981.4484199805</v>
       </c>
       <c r="B72">
-        <v>0.01167920946104795</v>
+        <v>0.01868577697361762</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>1578.4134969705</v>
+        <v>978.4134969705</v>
       </c>
       <c r="B73">
-        <v>0.01357587423403173</v>
+        <v>0.02172028500773548</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74">
-        <v>1581.0049411405</v>
+        <v>981.0049411405</v>
       </c>
       <c r="B74">
-        <v>0.01195636004793932</v>
+        <v>0.01912919517516909</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>1581.9234433405</v>
+        <v>981.9234433405001</v>
       </c>
       <c r="B75">
-        <v>0.01138234523408477</v>
+        <v>0.0182108185652613</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>1582.5816590705</v>
+        <v>982.5816590705</v>
       </c>
       <c r="B76">
-        <v>0.01097099556096226</v>
+        <v>0.01755269283545324</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77">
-        <v>1582.2525622505</v>
+        <v>982.2525622505</v>
       </c>
       <c r="B77">
-        <v>0.01117666349498847</v>
+        <v>0.01788174465686754</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>1583.0273910905</v>
+        <v>983.0273910905</v>
       </c>
       <c r="B78">
-        <v>0.010692436856923</v>
+        <v>0.01710702176198708</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>1584.2566112305</v>
+        <v>984.2566112305</v>
       </c>
       <c r="B79">
-        <v>0.009924239927347367</v>
+        <v>0.01587796969765509</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>1585.2512797505</v>
+        <v>985.2512797505</v>
       </c>
       <c r="B80">
-        <v>0.009302625231862871</v>
+        <v>0.01488343718224083</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>1584.6215380305</v>
+        <v>984.6215380305</v>
       </c>
       <c r="B81">
-        <v>0.009696180169654345</v>
+        <v>0.01551309279540214</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>1585.9141122905</v>
+        <v>985.9141122905</v>
       </c>
       <c r="B82">
-        <v>0.008888390299094162</v>
+        <v>0.01422069527370562</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>1586.4170795005</v>
+        <v>986.4170795005</v>
       </c>
       <c r="B83">
-        <v>0.00857406265848204</v>
+        <v>0.01371779683621188</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>1580.09536287989</v>
+        <v>980.09536287989</v>
       </c>
       <c r="B84">
-        <v>0.01252479787634109</v>
+        <v>0.02003864906588904</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>1581.54375487989</v>
+        <v>981.54375487989</v>
       </c>
       <c r="B85">
-        <v>0.0116196302411754</v>
+        <v>0.01859045510970958</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>1596.41184319989</v>
+        <v>996.41184319989</v>
       </c>
       <c r="B86">
-        <v>0.002327869209597377</v>
+        <v>0.003724399756624086</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>1595.74333311989</v>
+        <v>995.7433331198901</v>
       </c>
       <c r="B87">
-        <v>0.002745652301604284</v>
+        <v>0.004392818428848866</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>1599.22533375989</v>
+        <v>999.22533375989</v>
       </c>
       <c r="B88">
-        <v>0.0005695878902057805</v>
+        <v>0.0009112938952551275</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>1604.31474431989</v>
+        <v>1001.744994000435</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>1605.02280831989</v>
+        <v>1002.193421000435</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>1605.148634119283</v>
+        <v>1003.242609841435</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1126,47 +1126,47 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>1602.225537159283</v>
+        <v>1001.248183267569</v>
       </c>
       <c r="B92">
-        <v>0.00182107556762412</v>
+        <v>0.001987980329285821</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>1598.487999439283</v>
+        <v>998.8208028275689</v>
       </c>
       <c r="B93">
-        <v>0.004149543873022354</v>
+        <v>0.004407515161826248</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>1597.968673919283</v>
+        <v>998.4835217875689</v>
       </c>
       <c r="B94">
-        <v>0.00447308121340384</v>
+        <v>0.004743706065892028</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>1597.421526199283</v>
+        <v>998.1281713475689</v>
       </c>
       <c r="B95">
-        <v>0.00481395165267029</v>
+        <v>0.00509790796732057</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>1599.028483159283</v>
+        <v>999.1718252675689</v>
       </c>
       <c r="B96">
-        <v>0.003812825074207549</v>
+        <v>0.00405762727174197</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>1605.722204599283</v>
+        <v>1003.519128147569</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -1177,295 +1177,295 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>1602.690140480933</v>
+        <v>1001.271142429219</v>
       </c>
       <c r="B98">
-        <v>0.001888286846669529</v>
+        <v>0.002240102510551623</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>1587.771168500933</v>
+        <v>990.2741509292189</v>
       </c>
       <c r="B99">
-        <v>0.01117941574634318</v>
+        <v>0.01319852990027137</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>1585.366350320933</v>
+        <v>988.5015244292189</v>
       </c>
       <c r="B100">
-        <v>0.01267707092798787</v>
+        <v>0.01496494017614936</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>1585.831665710933</v>
+        <v>988.8445151792189</v>
       </c>
       <c r="B101">
-        <v>0.01238728519253052</v>
+        <v>0.01462315222176014</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102">
-        <v>1578.312865670933</v>
+        <v>983.302298179219</v>
       </c>
       <c r="B102">
-        <v>0.01706978881517696</v>
+        <v>0.02014593384549512</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103">
-        <v>1572.187168280933</v>
+        <v>978.7869574292189</v>
       </c>
       <c r="B103">
-        <v>0.02088470609816273</v>
+        <v>0.02464544025583637</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104">
-        <v>1577.617269590933</v>
+        <v>982.7895641792189</v>
       </c>
       <c r="B104">
-        <v>0.0175029870844714</v>
+        <v>0.02065686979640868</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105">
-        <v>1573.261707830933</v>
+        <v>979.5790161792189</v>
       </c>
       <c r="B105">
-        <v>0.02021551216977213</v>
+        <v>0.02385615908741257</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106">
-        <v>1578.047707430933</v>
+        <v>983.1068461792189</v>
       </c>
       <c r="B106">
-        <v>0.01723492213602196</v>
+        <v>0.02034070043690117</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107">
-        <v>1582.010685710933</v>
+        <v>986.0280151792189</v>
       </c>
       <c r="B107">
-        <v>0.01476688733607412</v>
+        <v>0.01742977535529133</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108">
-        <v>1581.555500360933</v>
+        <v>985.6924914292189</v>
       </c>
       <c r="B108">
-        <v>0.01505036435887186</v>
+        <v>0.01776412249486148</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109">
-        <v>1575.256881410933</v>
+        <v>981.0496876792189</v>
       </c>
       <c r="B109">
-        <v>0.01897297247374918</v>
+        <v>0.02239064491957121</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110">
-        <v>1599.519793400933</v>
+        <v>998.9342334292189</v>
       </c>
       <c r="B110">
-        <v>0.003862692550793967</v>
+        <v>0.00456881646771734</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111">
-        <v>1605.123305000933</v>
+        <v>1003.064663429219</v>
       </c>
       <c r="B111">
-        <v>0.0003729783374948337</v>
+        <v>0.000452871007241229</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112">
-        <v>1602.138501244133</v>
+        <v>1000.696820632419</v>
       </c>
       <c r="B112">
-        <v>0.002231832719809868</v>
+        <v>0.002812410282960642</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113">
-        <v>1594.142089384133</v>
+        <v>994.3811374124189</v>
       </c>
       <c r="B113">
-        <v>0.007211779959186648</v>
+        <v>0.009105945745167876</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114">
-        <v>1575.774315004133</v>
+        <v>979.8740001524189</v>
       </c>
       <c r="B114">
-        <v>0.0186507289426342</v>
+        <v>0.02356220956026744</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <v>1577.159675104133</v>
+        <v>980.9681778524189</v>
       </c>
       <c r="B115">
-        <v>0.01778796445196951</v>
+        <v>0.02247186890874475</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <v>1571.729652554133</v>
+        <v>976.6794665024189</v>
       </c>
       <c r="B116">
-        <v>0.02116963441608066</v>
+        <v>0.02674554066019075</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <v>1569.324527384133</v>
+        <v>974.7798634124189</v>
       </c>
       <c r="B117">
-        <v>0.02266748078272562</v>
+        <v>0.02863848224617382</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <v>1573.451322294133</v>
+        <v>978.0392664824188</v>
       </c>
       <c r="B118">
-        <v>0.0200974254529932</v>
+        <v>0.02539050920950969</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119">
-        <v>1591.295293854133</v>
+        <v>992.1326966024189</v>
       </c>
       <c r="B119">
-        <v>0.008984686581419266</v>
+        <v>0.0113465017514599</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <v>1577.293265384133</v>
+        <v>981.073689412419</v>
       </c>
       <c r="B120">
-        <v>0.01770476806867405</v>
+        <v>0.02236672735534473</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <v>1573.445431874133</v>
+        <v>978.0346141424189</v>
       </c>
       <c r="B121">
-        <v>0.02010109384593395</v>
+        <v>0.02539514523474273</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <v>1573.877710904133</v>
+        <v>978.3760344524189</v>
       </c>
       <c r="B122">
-        <v>0.01983188225456289</v>
+        <v>0.02505492221315442</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123">
-        <v>1568.153889764133</v>
+        <v>973.8552766724189</v>
       </c>
       <c r="B123">
-        <v>0.02339652196845943</v>
+        <v>0.02955982665712364</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <v>1578.679014474133</v>
+        <v>982.168174342419</v>
       </c>
       <c r="B124">
-        <v>0.01684176132564519</v>
+        <v>0.02127608055121211</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125">
-        <v>1576.506005194133</v>
+        <v>980.4518997824189</v>
       </c>
       <c r="B125">
-        <v>0.01819505224594009</v>
+        <v>0.02298633650135851</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
-        <v>1588.956640368333</v>
+        <v>990.7608083966189</v>
       </c>
       <c r="B126">
-        <v>0.01044113619586773</v>
+        <v>0.01271357903710413</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <v>1587.619826668333</v>
+        <v>989.6530394966189</v>
       </c>
       <c r="B127">
-        <v>0.01127366731250234</v>
+        <v>0.01381746322717914</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
-        <v>1593.343448038333</v>
+        <v>994.3959963866189</v>
       </c>
       <c r="B128">
-        <v>0.007709152009913955</v>
+        <v>0.009091138878230098</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129">
-        <v>1596.367605578333</v>
+        <v>996.9020057666189</v>
       </c>
       <c r="B129">
-        <v>0.005825789164623729</v>
+        <v>0.006593917540131722</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130">
-        <v>1590.335227581024</v>
+        <v>991.9664031293104</v>
       </c>
       <c r="B130">
-        <v>0.009582589674718145</v>
+        <v>0.01151221206872666</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131">
-        <v>1588.891185561024</v>
+        <v>990.8258775893104</v>
       </c>
       <c r="B131">
-        <v>0.0104818996648669</v>
+        <v>0.01264873802823208</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132">
-        <v>1596.459152721024</v>
+        <v>996.8031689093104</v>
       </c>
       <c r="B132">
-        <v>0.005768776100701922</v>
+        <v>0.006692407797602828</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133">
-        <v>1599.897458167184</v>
+        <v>999.6357145154705</v>
       </c>
       <c r="B133">
-        <v>0.003627493233521184</v>
+        <v>0.003869795326439829</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134">
-        <v>1607.353465667184</v>
+        <v>1005.79676041547</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135">
-        <v>1609.516898167184</v>
+        <v>1007.58444731547</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136">
-        <v>1610.849187917184</v>
+        <v>1008.68534458547</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137">
-        <v>1626.427583167184</v>
+        <v>1021.55807951547</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138">
-        <v>1628.407759417184</v>
+        <v>1023.19433816547</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139">
-        <v>1630.509927167184</v>
+        <v>1024.93140079547</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -1516,1826 +1516,1826 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140">
-        <v>1628.834395685316</v>
+        <v>1023.432925986848</v>
       </c>
       <c r="B140">
-        <v>0.001027611947619134</v>
+        <v>0.001462024490087588</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141">
-        <v>1625.588253085316</v>
+        <v>1020.186783386848</v>
       </c>
       <c r="B141">
-        <v>0.003018487652153956</v>
+        <v>0.00462920484721252</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142">
-        <v>1627.199497685316</v>
+        <v>1021.798027986848</v>
       </c>
       <c r="B142">
-        <v>0.002030303174921477</v>
+        <v>0.003057153684813185</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143">
-        <v>1626.214828525316</v>
+        <v>1020.813358826848</v>
       </c>
       <c r="B143">
-        <v>0.002634205759992403</v>
+        <v>0.004017870820843816</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144">
-        <v>1627.457621925316</v>
+        <v>1022.056152226848</v>
       </c>
       <c r="B144">
-        <v>0.001871994270633892</v>
+        <v>0.002805308302966658</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145">
-        <v>1627.818487365316</v>
+        <v>1022.417017666848</v>
       </c>
       <c r="B145">
-        <v>0.00165067366780447</v>
+        <v>0.00245322089524358</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146">
-        <v>1625.561598725316</v>
+        <v>1020.160129026848</v>
       </c>
       <c r="B146">
-        <v>0.003034834906197603</v>
+        <v>0.004655210841349566</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147">
-        <v>1620.711964005316</v>
+        <v>1015.310494306848</v>
       </c>
       <c r="B147">
-        <v>0.006009140452699624</v>
+        <v>0.00938687845952979</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148">
-        <v>1621.282396485316</v>
+        <v>1015.880926786848</v>
       </c>
       <c r="B148">
-        <v>0.005659291322378079</v>
+        <v>0.008830321718700795</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149">
-        <v>1618.797893365316</v>
+        <v>1013.396423666848</v>
       </c>
       <c r="B149">
-        <v>0.007183049674660213</v>
+        <v>0.01125438943491264</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150">
-        <v>1619.843978005316</v>
+        <v>1014.442508306848</v>
       </c>
       <c r="B150">
-        <v>0.006541480664517874</v>
+        <v>0.01023375074710564</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151">
-        <v>1618.603747925316</v>
+        <v>1013.202278226848</v>
       </c>
       <c r="B151">
-        <v>0.007302120056732253</v>
+        <v>0.01144381229760305</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152">
-        <v>1613.126162325316</v>
+        <v>1007.724692626848</v>
       </c>
       <c r="B152">
-        <v>0.01066155105971722</v>
+        <v>0.01678815592464844</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153">
-        <v>1614.260879485316</v>
+        <v>1008.859409786848</v>
       </c>
       <c r="B153">
-        <v>0.009965623275964619</v>
+        <v>0.01568104069808862</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154">
-        <v>1616.496698885316</v>
+        <v>1011.095229186848</v>
       </c>
       <c r="B154">
-        <v>0.008594383909219627</v>
+        <v>0.01349960748386092</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155">
-        <v>1613.984624445316</v>
+        <v>1008.583154746848</v>
       </c>
       <c r="B155">
-        <v>0.01013505189175967</v>
+        <v>0.01595057584920756</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156">
-        <v>1615.254864125316</v>
+        <v>1009.853394426848</v>
       </c>
       <c r="B156">
-        <v>0.009356007459808913</v>
+        <v>0.01471123468060431</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157">
-        <v>1614.893936165316</v>
+        <v>1009.492466466848</v>
       </c>
       <c r="B157">
-        <v>0.009577366406471111</v>
+        <v>0.01506338308753175</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158">
-        <v>1613.433906605316</v>
+        <v>1008.032436906848</v>
       </c>
       <c r="B158">
-        <v>0.01047280993347655</v>
+        <v>0.01648789750758639</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159">
-        <v>1615.774259445316</v>
+        <v>1010.372789746848</v>
       </c>
       <c r="B159">
-        <v>0.009037459678316706</v>
+        <v>0.01420447362362343</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160">
-        <v>1617.216491645316</v>
+        <v>1011.815021946848</v>
       </c>
       <c r="B160">
-        <v>0.008152931362377158</v>
+        <v>0.01279732364375108</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161">
-        <v>1616.935172485316</v>
+        <v>1011.533702786848</v>
       </c>
       <c r="B161">
-        <v>0.008325465828627698</v>
+        <v>0.01307179973042538</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162">
-        <v>1615.105045365316</v>
+        <v>1009.703575666848</v>
       </c>
       <c r="B162">
-        <v>0.00944789206443708</v>
+        <v>0.01485740910738431</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163">
-        <v>1613.498635645316</v>
+        <v>1008.097165946848</v>
       </c>
       <c r="B163">
-        <v>0.01043311128526747</v>
+        <v>0.01642474299797758</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164">
-        <v>1612.940998925316</v>
+        <v>1007.539529226848</v>
       </c>
       <c r="B164">
-        <v>0.01077511271114584</v>
+        <v>0.01696881523497529</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165">
-        <v>1612.958775445316</v>
+        <v>1007.557305746848</v>
       </c>
       <c r="B165">
-        <v>0.01076421028135754</v>
+        <v>0.01695147112786122</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166">
-        <v>1614.992655245316</v>
+        <v>1009.591185546848</v>
       </c>
       <c r="B166">
-        <v>0.009516821494505057</v>
+        <v>0.01496706534380432</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167">
-        <v>1610.171467125316</v>
+        <v>1004.769997426848</v>
       </c>
       <c r="B167">
-        <v>0.01247368059709042</v>
+        <v>0.01967097832398834</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168">
-        <v>1612.511945005316</v>
+        <v>1007.110475306848</v>
       </c>
       <c r="B168">
-        <v>0.01103825365426503</v>
+        <v>0.01738743244161656</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169">
-        <v>1613.567178405316</v>
+        <v>1008.165708706848</v>
       </c>
       <c r="B169">
-        <v>0.01039107366325864</v>
+        <v>0.01635786753690105</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170">
-        <v>1611.178997765316</v>
+        <v>1005.777528066848</v>
       </c>
       <c r="B170">
-        <v>0.01185575695049812</v>
+        <v>0.01868795581222016</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171">
-        <v>1609.167291725316</v>
+        <v>1003.765822026848</v>
       </c>
       <c r="B171">
-        <v>0.01308954645798999</v>
+        <v>0.02065072721178773</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172">
-        <v>1610.912745925316</v>
+        <v>1005.511276226848</v>
       </c>
       <c r="B172">
-        <v>0.01201905055304775</v>
+        <v>0.01894773109063719</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173">
-        <v>1611.031137965316</v>
+        <v>1005.629668266848</v>
       </c>
       <c r="B173">
-        <v>0.01194644011503243</v>
+        <v>0.01883221893059595</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174">
-        <v>1609.371836325316</v>
+        <v>1003.970366626848</v>
       </c>
       <c r="B174">
-        <v>0.01296409821839817</v>
+        <v>0.02045115814810095</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175">
-        <v>1613.458664525316</v>
+        <v>1008.057194826848</v>
       </c>
       <c r="B175">
-        <v>0.01045762577569409</v>
+        <v>0.01646374182264909</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176">
-        <v>1606.921094005316</v>
+        <v>1001.519624306848</v>
       </c>
       <c r="B176">
-        <v>0.01446715090097705</v>
+        <v>0.02284228629394347</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177">
-        <v>1605.797401205316</v>
+        <v>1000.395931506848</v>
       </c>
       <c r="B177">
-        <v>0.0151563173888819</v>
+        <v>0.02393864532746315</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178">
-        <v>1604.669165285316</v>
+        <v>999.2676955868477</v>
       </c>
       <c r="B178">
-        <v>0.01584827019530266</v>
+        <v>0.02503943696983479</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179">
-        <v>1601.680730125316</v>
+        <v>996.2792604268477</v>
       </c>
       <c r="B179">
-        <v>0.01768109262110162</v>
+        <v>0.02795517860647567</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180">
-        <v>1593.423734565316</v>
+        <v>988.0222648668476</v>
       </c>
       <c r="B180">
-        <v>0.02274514983561082</v>
+        <v>0.03601132319682743</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181">
-        <v>1595.384340925316</v>
+        <v>989.9828712268477</v>
       </c>
       <c r="B181">
-        <v>0.02154270002078129</v>
+        <v>0.03409840848031231</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182">
-        <v>1591.397315485316</v>
+        <v>985.9958457868477</v>
       </c>
       <c r="B182">
-        <v>0.02398796292508454</v>
+        <v>0.03798844974249405</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183">
-        <v>1591.242703525316</v>
+        <v>985.8412338268477</v>
       </c>
       <c r="B183">
-        <v>0.02408278722355939</v>
+        <v>0.03813930077494365</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184">
-        <v>1591.778916725316</v>
+        <v>986.3774470268477</v>
       </c>
       <c r="B184">
-        <v>0.02375392495104833</v>
+        <v>0.03761613093198257</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185">
-        <v>1593.445470685316</v>
+        <v>988.0440009868477</v>
       </c>
       <c r="B185">
-        <v>0.02273181896307963</v>
+        <v>0.03599011580676881</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186">
-        <v>1596.034111285316</v>
+        <v>990.6326415868477</v>
       </c>
       <c r="B186">
-        <v>0.02114419256665689</v>
+        <v>0.03346444374911595</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187">
-        <v>1593.002141365316</v>
+        <v>987.6006716668477</v>
       </c>
       <c r="B187">
-        <v>0.02300371508135124</v>
+        <v>0.03642266116507853</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188">
-        <v>1594.191938645316</v>
+        <v>988.7904689468477</v>
       </c>
       <c r="B188">
-        <v>0.02227400638091603</v>
+        <v>0.03526180563945347</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189">
-        <v>1590.587431405316</v>
+        <v>985.1859617068477</v>
       </c>
       <c r="B189">
-        <v>0.02448466893496892</v>
+        <v>0.03877863343612598</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190">
-        <v>1593.929979845316</v>
+        <v>988.5285101468477</v>
       </c>
       <c r="B190">
-        <v>0.02243466704028096</v>
+        <v>0.03551739230583595</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191">
-        <v>1591.599609365316</v>
+        <v>986.1981396668477</v>
       </c>
       <c r="B191">
-        <v>0.02386389506347297</v>
+        <v>0.03779107665016501</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192">
-        <v>1592.108209565316</v>
+        <v>986.7067398668477</v>
       </c>
       <c r="B192">
-        <v>0.02355196798377479</v>
+        <v>0.03729484812247508</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193">
-        <v>1593.877275485316</v>
+        <v>988.4758057868477</v>
       </c>
       <c r="B193">
-        <v>0.02246699089131787</v>
+        <v>0.03556881463513439</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194">
-        <v>1591.408173125316</v>
+        <v>986.0067034268477</v>
       </c>
       <c r="B194">
-        <v>0.02398130387945763</v>
+        <v>0.03797785621399874</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195">
-        <v>1592.544849245316</v>
+        <v>987.1433795468477</v>
       </c>
       <c r="B195">
-        <v>0.02328417465561128</v>
+        <v>0.03686882967903482</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196">
-        <v>1592.310545125316</v>
+        <v>986.9090754268477</v>
       </c>
       <c r="B196">
-        <v>0.02342787455960815</v>
+        <v>0.03709743436400992</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197">
-        <v>1591.600317925316</v>
+        <v>986.1988482268476</v>
       </c>
       <c r="B197">
-        <v>0.02386346050003474</v>
+        <v>0.03779038532584877</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198">
-        <v>1590.409207725316</v>
+        <v>985.0077380268477</v>
       </c>
       <c r="B198">
-        <v>0.02459397442095856</v>
+        <v>0.03895252183476583</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199">
-        <v>1591.245996245316</v>
+        <v>985.8445265468476</v>
       </c>
       <c r="B199">
-        <v>0.02408076778169943</v>
+        <v>0.03813608815017921</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200">
-        <v>1592.156224925316</v>
+        <v>986.7547552268477</v>
       </c>
       <c r="B200">
-        <v>0.02352251992019672</v>
+        <v>0.03724800073350565</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201">
-        <v>1596.878819005316</v>
+        <v>991.4773493068477</v>
       </c>
       <c r="B201">
-        <v>0.02062612904191186</v>
+        <v>0.03264028349864034</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202">
-        <v>1597.018071885316</v>
+        <v>991.6166021868477</v>
       </c>
       <c r="B202">
-        <v>0.0205407245450242</v>
+        <v>0.03250441793740189</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203">
-        <v>1589.706009491516</v>
+        <v>984.3045397930478</v>
       </c>
       <c r="B203">
-        <v>0.02502524946079931</v>
+        <v>0.0396386148096266</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204">
-        <v>1592.060325091516</v>
+        <v>986.6588553930477</v>
       </c>
       <c r="B204">
-        <v>0.02358133577418342</v>
+        <v>0.03734156780904418</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205">
-        <v>1589.321552691516</v>
+        <v>983.9200829930477</v>
       </c>
       <c r="B205">
-        <v>0.02526103876425234</v>
+        <v>0.04001371971879575</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206">
-        <v>1589.917893891516</v>
+        <v>984.5164241930477</v>
       </c>
       <c r="B206">
-        <v>0.02489529968467741</v>
+        <v>0.03943188448617718</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207">
-        <v>1590.118712691516</v>
+        <v>984.7172429930476</v>
       </c>
       <c r="B207">
-        <v>0.02477213649710408</v>
+        <v>0.0392359505926072</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208">
-        <v>1595.410872291516</v>
+        <v>990.0094025930478</v>
       </c>
       <c r="B208">
-        <v>0.02152642819945838</v>
+        <v>0.03407252248815773</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209">
-        <v>1594.508989491516</v>
+        <v>989.1075197930477</v>
       </c>
       <c r="B209">
-        <v>0.02207955749046919</v>
+        <v>0.03495246703791011</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210">
-        <v>1589.644987332716</v>
+        <v>984.2435176342477</v>
       </c>
       <c r="B210">
-        <v>0.02506267465998602</v>
+        <v>0.03969815260771981</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211">
-        <v>1589.148974132716</v>
+        <v>983.7475044342477</v>
       </c>
       <c r="B211">
-        <v>0.02536688206880666</v>
+        <v>0.04018210031350289</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212">
-        <v>1583.824572632716</v>
+        <v>978.4231029342477</v>
       </c>
       <c r="B212">
-        <v>0.0286323644870895</v>
+        <v>0.04537698603548157</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213">
-        <v>1580.335221232716</v>
+        <v>974.9337515342477</v>
       </c>
       <c r="B213">
-        <v>0.03077240138098469</v>
+        <v>0.04878145915172327</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214">
-        <v>1570.658832132716</v>
+        <v>965.2573624342477</v>
       </c>
       <c r="B214">
-        <v>0.03670697984553384</v>
+        <v>0.05822247061111441</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215">
-        <v>1549.283194532716</v>
+        <v>943.8817248342477</v>
       </c>
       <c r="B215">
-        <v>0.04981676669432511</v>
+        <v>0.07907814698458682</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216">
-        <v>1547.447464532716</v>
+        <v>942.0459948342477</v>
       </c>
       <c r="B216">
-        <v>0.05094262920482773</v>
+        <v>0.08086922295179322</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217">
-        <v>1549.786895832716</v>
+        <v>944.3854261342477</v>
       </c>
       <c r="B217">
-        <v>0.04950784413481946</v>
+        <v>0.07858669819141972</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218">
-        <v>1538.372891532716</v>
+        <v>932.9714218342477</v>
       </c>
       <c r="B218">
-        <v>0.05650811080589113</v>
+        <v>0.0897230574552117</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219">
-        <v>1538.725916532716</v>
+        <v>933.3244468342477</v>
       </c>
       <c r="B219">
-        <v>0.05629159878464052</v>
+        <v>0.08937861976921047</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220">
-        <v>1530.891271932716</v>
+        <v>925.4898022342477</v>
       </c>
       <c r="B220">
-        <v>0.06109662601536203</v>
+        <v>0.09702268706378203</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221">
-        <v>1539.276060232716</v>
+        <v>933.8745905342477</v>
       </c>
       <c r="B221">
-        <v>0.05595419286589465</v>
+        <v>0.08884185828490732</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222">
-        <v>1539.275484932716</v>
+        <v>933.8740152342477</v>
       </c>
       <c r="B222">
-        <v>0.05595454570029967</v>
+        <v>0.08884241959076589</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223">
-        <v>1540.058049832716</v>
+        <v>934.6565801342477</v>
       </c>
       <c r="B223">
-        <v>0.05547459468193361</v>
+        <v>0.08807889053956053</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224">
-        <v>1536.211227932716</v>
+        <v>930.8097582342477</v>
       </c>
       <c r="B224">
-        <v>0.05783387004475415</v>
+        <v>0.09183213870525664</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225">
-        <v>1542.080020132716</v>
+        <v>936.6785504342477</v>
       </c>
       <c r="B225">
-        <v>0.05423451005177571</v>
+        <v>0.08610610455756151</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226">
-        <v>1542.747158932716</v>
+        <v>937.3456892342477</v>
       </c>
       <c r="B226">
-        <v>0.05382535044539472</v>
+        <v>0.08545519387272704</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227">
-        <v>1544.072963932716</v>
+        <v>938.6714942342477</v>
       </c>
       <c r="B227">
-        <v>0.05301222752114265</v>
+        <v>0.08416163900752249</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228">
-        <v>1541.703146332716</v>
+        <v>936.3016766342477</v>
       </c>
       <c r="B228">
-        <v>0.05446564866290615</v>
+        <v>0.08647381092279482</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229">
-        <v>1540.157629032716</v>
+        <v>934.7561593342477</v>
       </c>
       <c r="B229">
-        <v>0.05541352225401341</v>
+        <v>0.08798173359820549</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230">
-        <v>1537.745186932716</v>
+        <v>932.3437172342477</v>
       </c>
       <c r="B230">
-        <v>0.05689308521760206</v>
+        <v>0.09033549317482459</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231">
-        <v>1536.481717409516</v>
+        <v>931.0802477110477</v>
       </c>
       <c r="B231">
-        <v>0.0576679774780835</v>
+        <v>0.09156822887032523</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232">
-        <v>1535.094981409516</v>
+        <v>929.6935117110477</v>
       </c>
       <c r="B232">
-        <v>0.05851846969336805</v>
+        <v>0.09292123259225604</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233">
-        <v>1530.014296709516</v>
+        <v>924.6128270110478</v>
       </c>
       <c r="B233">
-        <v>0.06163447936331656</v>
+        <v>0.09787832991219048</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234">
-        <v>1529.807283409516</v>
+        <v>924.4058137110477</v>
       </c>
       <c r="B234">
-        <v>0.061761441669127</v>
+        <v>0.09808030762488362</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235">
-        <v>1530.290646809516</v>
+        <v>924.8891771110477</v>
       </c>
       <c r="B235">
-        <v>0.06146499244674186</v>
+        <v>0.09760870201340088</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236">
-        <v>1537.353796409516</v>
+        <v>931.9523267110477</v>
       </c>
       <c r="B236">
-        <v>0.05713312700862627</v>
+        <v>0.09071736314475265</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237">
-        <v>1536.886846809516</v>
+        <v>931.4853771110477</v>
       </c>
       <c r="B237">
-        <v>0.05741950956430397</v>
+        <v>0.09117295422103111</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238">
-        <v>1539.868022409516</v>
+        <v>934.4665527110477</v>
       </c>
       <c r="B238">
-        <v>0.05559113946343652</v>
+        <v>0.08826429555598647</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239">
-        <v>1548.001827309516</v>
+        <v>942.6003576110477</v>
       </c>
       <c r="B239">
-        <v>0.05060263570490287</v>
+        <v>0.08032834501950459</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240">
-        <v>1547.769963209516</v>
+        <v>942.3684935110477</v>
       </c>
       <c r="B240">
-        <v>0.05074483913227035</v>
+        <v>0.08055456903783398</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241">
-        <v>1547.747566809516</v>
+        <v>942.3460971110477</v>
       </c>
       <c r="B241">
-        <v>0.05075857495787117</v>
+        <v>0.08057642064661741</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242">
-        <v>1542.153375609516</v>
+        <v>937.2157914154457</v>
       </c>
       <c r="B242">
-        <v>0.05418952076616756</v>
+        <v>0.08558193193412444</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243">
-        <v>1535.259119409516</v>
+        <v>932.5147536154457</v>
       </c>
       <c r="B243">
-        <v>0.0584178030262934</v>
+        <v>0.09016861724433289</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244">
-        <v>1530.389743209516</v>
+        <v>929.1944358154457</v>
       </c>
       <c r="B244">
-        <v>0.06140421612250802</v>
+        <v>0.09340816849373657</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245">
-        <v>1539.603385932716</v>
+        <v>936.1971457386456</v>
       </c>
       <c r="B245">
-        <v>0.05575344235555069</v>
+        <v>0.08657579911002455</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246">
-        <v>1543.224499032716</v>
+        <v>938.9545720386457</v>
       </c>
       <c r="B246">
-        <v>0.05353259534341914</v>
+        <v>0.08388544705537981</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247">
-        <v>1545.691975032716</v>
+        <v>940.8335200386457</v>
       </c>
       <c r="B247">
-        <v>0.05201927981010801</v>
+        <v>0.08205220436368188</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248">
-        <v>1549.431653832716</v>
+        <v>943.6812324386457</v>
       </c>
       <c r="B248">
-        <v>0.04972571585340324</v>
+        <v>0.07927376241352813</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249">
-        <v>1545.397678323009</v>
+        <v>940.6170105289391</v>
       </c>
       <c r="B249">
-        <v>0.05219977347334981</v>
+        <v>0.08226344729129498</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250">
-        <v>1557.933679723009</v>
+        <v>949.1650271289391</v>
       </c>
       <c r="B250">
-        <v>0.04451138029577506</v>
+        <v>0.07392336073197436</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251">
-        <v>1565.327866523009</v>
+        <v>954.206956328939</v>
       </c>
       <c r="B251">
-        <v>0.03997648806555942</v>
+        <v>0.06900407618660209</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252">
-        <v>1563.578508637809</v>
+        <v>952.880499243739</v>
       </c>
       <c r="B252">
-        <v>0.04104937812041443</v>
+        <v>0.07029826727506949</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253">
-        <v>1562.177706833828</v>
+        <v>952.3581962937391</v>
       </c>
       <c r="B253">
-        <v>0.0419084969645509</v>
+        <v>0.07080786523410809</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254">
-        <v>1558.744947633828</v>
+        <v>948.9254370937391</v>
       </c>
       <c r="B254">
-        <v>0.04401382557543765</v>
+        <v>0.0741571227525486</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255">
-        <v>1557.027980433828</v>
+        <v>947.208469893739</v>
       </c>
       <c r="B255">
-        <v>0.04506685025893831</v>
+        <v>0.07583232481843083</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256">
-        <v>1557.972620883828</v>
+        <v>948.1531103437391</v>
       </c>
       <c r="B256">
-        <v>0.04448749748453285</v>
+        <v>0.07491066269619806</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257">
-        <v>1548.653431783828</v>
+        <v>938.833921243739</v>
       </c>
       <c r="B257">
-        <v>0.05020300337917705</v>
+        <v>0.084003163026237</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258">
-        <v>1548.240422433828</v>
+        <v>938.420911893739</v>
       </c>
       <c r="B258">
-        <v>0.05045630410621871</v>
+        <v>0.08440612594617436</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259">
-        <v>1564.613567502068</v>
+        <v>954.7940569619791</v>
       </c>
       <c r="B259">
-        <v>0.04041457127440051</v>
+        <v>0.06843125674465267</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260">
-        <v>1573.227180542068</v>
+        <v>963.4076700019791</v>
       </c>
       <c r="B260">
-        <v>0.03513179875245387</v>
+        <v>0.06002716937518104</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261">
-        <v>1572.558002402068</v>
+        <v>962.738491861979</v>
       </c>
       <c r="B261">
-        <v>0.03554220909639005</v>
+        <v>0.06068006979318052</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262">
-        <v>1571.298190882068</v>
+        <v>961.478680341979</v>
       </c>
       <c r="B262">
-        <v>0.03631485788497413</v>
+        <v>0.06190923646621072</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263">
-        <v>1568.00947088877</v>
+        <v>958.1899603486811</v>
       </c>
       <c r="B263">
-        <v>0.03833184652055499</v>
+        <v>0.06511795852384838</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264">
-        <v>1567.82356893877</v>
+        <v>958.0040583986811</v>
       </c>
       <c r="B264">
-        <v>0.03844586112844084</v>
+        <v>0.0652993384189865</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265">
-        <v>1565.76535303877</v>
+        <v>955.945842498681</v>
       </c>
       <c r="B265">
-        <v>0.0397081753687325</v>
+        <v>0.06730748832872935</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266">
-        <v>1564.11071775148</v>
+        <v>954.291207211391</v>
       </c>
       <c r="B266">
-        <v>0.04072297157433713</v>
+        <v>0.06892187470230116</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267">
-        <v>1562.254903531481</v>
+        <v>952.435392991391</v>
       </c>
       <c r="B267">
-        <v>0.04186115183873107</v>
+        <v>0.07073254634194415</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268">
-        <v>1568.80320465148</v>
+        <v>958.9836941113911</v>
       </c>
       <c r="B268">
-        <v>0.03784504558209711</v>
+        <v>0.06434353229191336</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269">
-        <v>1565.40092607148</v>
+        <v>955.581415531391</v>
       </c>
       <c r="B269">
-        <v>0.03993168027429495</v>
+        <v>0.06766305062978395</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270">
-        <v>1567.49219571148</v>
+        <v>957.6726851713911</v>
       </c>
       <c r="B270">
-        <v>0.03864909400778049</v>
+        <v>0.06562265101047582</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271">
-        <v>1573.52921949148</v>
+        <v>963.7097089513911</v>
       </c>
       <c r="B271">
-        <v>0.03494655673437141</v>
+        <v>0.05973247750684962</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272">
-        <v>1567.26006459148</v>
+        <v>957.440554051391</v>
       </c>
       <c r="B272">
-        <v>0.03879146119986709</v>
+        <v>0.06584913555355831</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273">
-        <v>1574.89740639148</v>
+        <v>965.0778958513911</v>
       </c>
       <c r="B273">
-        <v>0.03410744077610361</v>
+        <v>0.05839757167906634</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274">
-        <v>1574.71067571148</v>
+        <v>964.8911651713911</v>
       </c>
       <c r="B274">
-        <v>0.03422196364829766</v>
+        <v>0.05857976014539201</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275">
-        <v>1579.16799213148</v>
+        <v>969.3484815913911</v>
       </c>
       <c r="B275">
-        <v>0.03148826890303236</v>
+        <v>0.05423086770581942</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276">
-        <v>1579.52606673148</v>
+        <v>969.7065561913911</v>
       </c>
       <c r="B276">
-        <v>0.03126865993651584</v>
+        <v>0.05388150325106456</v>
       </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277">
-        <v>1577.74414460452</v>
+        <v>967.9246340644308</v>
       </c>
       <c r="B277">
-        <v>0.03236152180584284</v>
+        <v>0.05562008021882769</v>
       </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278">
-        <v>1576.64364800452</v>
+        <v>966.8241374644309</v>
       </c>
       <c r="B278">
-        <v>0.03303646194675447</v>
+        <v>0.05669380729865547</v>
       </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279">
-        <v>1575.38802960452</v>
+        <v>965.5685190644309</v>
       </c>
       <c r="B279">
-        <v>0.03380653907359621</v>
+        <v>0.05791888284910263</v>
       </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280">
-        <v>1571.59485794327</v>
+        <v>961.7753474031809</v>
       </c>
       <c r="B280">
-        <v>0.03613291047314993</v>
+        <v>0.06161978581519967</v>
       </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281">
-        <v>1570.48844264327</v>
+        <v>960.668932103181</v>
       </c>
       <c r="B281">
-        <v>0.03681148058276118</v>
+        <v>0.06269928762297061</v>
       </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282">
-        <v>1553.27194559327</v>
+        <v>943.4524350531809</v>
       </c>
       <c r="B282">
-        <v>0.04737044545819225</v>
+        <v>0.07949699431498725</v>
       </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283">
-        <v>1555.50493799327</v>
+        <v>945.6854274531809</v>
       </c>
       <c r="B283">
-        <v>0.04600093990487153</v>
+        <v>0.07731831933413791</v>
       </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284">
-        <v>1558.24825769327</v>
+        <v>948.4287471531809</v>
       </c>
       <c r="B284">
-        <v>0.0443184480326716</v>
+        <v>0.07464173073721247</v>
       </c>
     </row>
     <row r="285" spans="1:2">
       <c r="A285">
-        <v>1557.40248479327</v>
+        <v>947.582974253181</v>
       </c>
       <c r="B285">
-        <v>0.04483716483770783</v>
+        <v>0.07546693025724227</v>
       </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286">
-        <v>1558.34694824327</v>
+        <v>948.5274377031809</v>
       </c>
       <c r="B286">
-        <v>0.04425792061829925</v>
+        <v>0.07454544082949432</v>
       </c>
     </row>
     <row r="287" spans="1:2">
       <c r="A287">
-        <v>1557.17055104327</v>
+        <v>947.3510405031809</v>
       </c>
       <c r="B287">
-        <v>0.04497941098177327</v>
+        <v>0.07569322223133934</v>
       </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288">
-        <v>1558.56551384327</v>
+        <v>948.7460033031809</v>
       </c>
       <c r="B288">
-        <v>0.04412387322836409</v>
+        <v>0.07433219182587281</v>
       </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289">
-        <v>1548.93759689327</v>
+        <v>939.1180863531808</v>
       </c>
       <c r="B289">
-        <v>0.0500287234777137</v>
+        <v>0.08372591021768683</v>
       </c>
     </row>
     <row r="290" spans="1:2">
       <c r="A290">
-        <v>1547.45139464327</v>
+        <v>937.6318841031809</v>
       </c>
       <c r="B290">
-        <v>0.05094021884811106</v>
+        <v>0.0851759606784751</v>
       </c>
     </row>
     <row r="291" spans="1:2">
       <c r="A291">
-        <v>1543.93045769327</v>
+        <v>934.1109471531809</v>
       </c>
       <c r="B291">
-        <v>0.05309962731986273</v>
+        <v>0.08861125102792433</v>
       </c>
     </row>
     <row r="292" spans="1:2">
       <c r="A292">
-        <v>1549.26398429327</v>
+        <v>939.4444737531809</v>
       </c>
       <c r="B292">
-        <v>0.04982854843151374</v>
+        <v>0.0834074621735087</v>
       </c>
     </row>
     <row r="293" spans="1:2">
       <c r="A293">
-        <v>1545.80090294327</v>
+        <v>935.9813924031808</v>
       </c>
       <c r="B293">
-        <v>0.0519524737706355</v>
+        <v>0.08678630425729328</v>
       </c>
     </row>
     <row r="294" spans="1:2">
       <c r="A294">
-        <v>1547.54212274327</v>
+        <v>937.7226122031809</v>
       </c>
       <c r="B294">
-        <v>0.0508845748446688</v>
+        <v>0.08508743953459219</v>
       </c>
     </row>
     <row r="295" spans="1:2">
       <c r="A295">
-        <v>1548.13704194327</v>
+        <v>938.317531403181</v>
       </c>
       <c r="B295">
-        <v>0.0505197078848989</v>
+        <v>0.08450699171190057</v>
       </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296">
-        <v>1546.82506394327</v>
+        <v>937.0055534031809</v>
       </c>
       <c r="B296">
-        <v>0.05132435063999052</v>
+        <v>0.08578705591813107</v>
       </c>
     </row>
     <row r="297" spans="1:2">
       <c r="A297">
-        <v>1545.94875614327</v>
+        <v>936.1292456031809</v>
       </c>
       <c r="B297">
-        <v>0.05186179465391483</v>
+        <v>0.08664204757837279</v>
       </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298">
-        <v>1547.17891814327</v>
+        <v>937.3594076031809</v>
       </c>
       <c r="B298">
-        <v>0.05110733006617851</v>
+        <v>0.08544180920237499</v>
       </c>
     </row>
     <row r="299" spans="1:2">
       <c r="A299">
-        <v>1545.69264284327</v>
+        <v>935.8731323031809</v>
       </c>
       <c r="B299">
-        <v>0.05201887023851115</v>
+        <v>0.08689193093622605</v>
       </c>
     </row>
     <row r="300" spans="1:2">
       <c r="A300">
-        <v>1538.34213269327</v>
+        <v>928.5226221531809</v>
       </c>
       <c r="B300">
-        <v>0.05652697535797557</v>
+        <v>0.09406364032506431</v>
       </c>
     </row>
     <row r="301" spans="1:2">
       <c r="A301">
-        <v>1542.01092284327</v>
+        <v>932.1914123031809</v>
       </c>
       <c r="B301">
-        <v>0.05427688776950312</v>
+        <v>0.09048409329669482</v>
       </c>
     </row>
     <row r="302" spans="1:2">
       <c r="A302">
-        <v>1542.20764649327</v>
+        <v>932.3881359531808</v>
       </c>
       <c r="B302">
-        <v>0.05415623615817455</v>
+        <v>0.09029215493882303</v>
       </c>
     </row>
     <row r="303" spans="1:2">
       <c r="A303">
-        <v>1557.11233019327</v>
+        <v>947.2928196531809</v>
       </c>
       <c r="B303">
-        <v>0.04501511812407888</v>
+        <v>0.07575002686231735</v>
       </c>
     </row>
     <row r="304" spans="1:2">
       <c r="A304">
-        <v>1559.21785034327</v>
+        <v>949.3983398031809</v>
       </c>
       <c r="B304">
-        <v>0.04372379194757514</v>
+        <v>0.07369572337589303</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="A305">
-        <v>1560.52201199327</v>
+        <v>950.7025014531808</v>
       </c>
       <c r="B305">
-        <v>0.0429239429995435</v>
+        <v>0.07242328538737219</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="A306">
-        <v>1564.67760734327</v>
+        <v>954.858096803181</v>
       </c>
       <c r="B306">
-        <v>0.04037529531530659</v>
+        <v>0.06836877466911839</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307">
-        <v>1548.44465549327</v>
+        <v>938.6251449531809</v>
       </c>
       <c r="B307">
-        <v>0.05033104693602986</v>
+        <v>0.08420686084483842</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="A308">
-        <v>1548.91358707341</v>
+        <v>939.0940765333208</v>
       </c>
       <c r="B308">
-        <v>0.0500434488218896</v>
+        <v>0.08374933599997958</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="A309">
-        <v>1543.79229593341</v>
+        <v>933.9727853933209</v>
       </c>
       <c r="B309">
-        <v>0.05318436262723991</v>
+        <v>0.08874605201046104</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="A310">
-        <v>1544.78195229341</v>
+        <v>934.9624417533209</v>
       </c>
       <c r="B310">
-        <v>0.05257740136713918</v>
+        <v>0.08778046898780023</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="A311">
-        <v>1547.81005485341</v>
+        <v>937.9905443133209</v>
       </c>
       <c r="B311">
-        <v>0.05072025072392849</v>
+        <v>0.08482602485851531</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312">
-        <v>1541.00443533341</v>
+        <v>931.184924793321</v>
       </c>
       <c r="B312">
-        <v>0.05489417165909505</v>
+        <v>0.09146609805240702</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="A313">
-        <v>1542.18359205341</v>
+        <v>932.3640815133209</v>
       </c>
       <c r="B313">
-        <v>0.05417098886802263</v>
+        <v>0.09031562425573658</v>
       </c>
     </row>
     <row r="314" spans="1:2">
       <c r="A314">
-        <v>1535.72360089341</v>
+        <v>925.904090353321</v>
       </c>
       <c r="B314">
-        <v>0.05813293417872889</v>
+        <v>0.09661847648075983</v>
       </c>
     </row>
     <row r="315" spans="1:2">
       <c r="A315">
-        <v>1531.68730177341</v>
+        <v>921.8677912333209</v>
       </c>
       <c r="B315">
-        <v>0.060608416880642</v>
+        <v>0.1005565928433452</v>
       </c>
     </row>
     <row r="316" spans="1:2">
       <c r="A316">
-        <v>1540.86245643341</v>
+        <v>931.042945893321</v>
       </c>
       <c r="B316">
-        <v>0.05498124803786131</v>
+        <v>0.09160462332335673</v>
       </c>
     </row>
     <row r="317" spans="1:2">
       <c r="A317">
-        <v>1539.77229267341</v>
+        <v>929.9527821333209</v>
       </c>
       <c r="B317">
-        <v>0.05564985099564512</v>
+        <v>0.09266826890895785</v>
       </c>
     </row>
     <row r="318" spans="1:2">
       <c r="A318">
-        <v>1536.16758989341</v>
+        <v>926.3480793533209</v>
       </c>
       <c r="B318">
-        <v>0.05786063347537085</v>
+        <v>0.09618528748913036</v>
       </c>
     </row>
     <row r="319" spans="1:2">
       <c r="A319">
-        <v>1535.06376493341</v>
+        <v>925.2442543933209</v>
       </c>
       <c r="B319">
-        <v>0.05853761491633491</v>
+        <v>0.09726226196678156</v>
       </c>
     </row>
     <row r="320" spans="1:2">
       <c r="A320">
-        <v>1539.16641845341</v>
+        <v>929.3469079133209</v>
       </c>
       <c r="B320">
-        <v>0.05602143672468929</v>
+        <v>0.09325940527138143</v>
       </c>
     </row>
     <row r="321" spans="1:2">
       <c r="A321">
-        <v>1537.71550143341</v>
+        <v>927.8959908933209</v>
       </c>
       <c r="B321">
-        <v>0.05691129148474017</v>
+        <v>0.09467502881347789</v>
       </c>
     </row>
     <row r="322" spans="1:2">
       <c r="A322">
-        <v>1540.97164845341</v>
+        <v>931.1521379133209</v>
       </c>
       <c r="B322">
-        <v>0.05491428001872767</v>
+        <v>0.09149808739332743</v>
       </c>
     </row>
     <row r="323" spans="1:2">
       <c r="A323">
-        <v>1542.71530547341</v>
+        <v>932.8957949333209</v>
       </c>
       <c r="B323">
-        <v>0.05384488633338569</v>
+        <v>0.08979684473587091</v>
       </c>
     </row>
     <row r="324" spans="1:2">
       <c r="A324">
-        <v>1541.06717927341</v>
+        <v>931.2476687333209</v>
       </c>
       <c r="B324">
-        <v>0.05485569048277428</v>
+        <v>0.09140488035534833</v>
       </c>
     </row>
     <row r="325" spans="1:2">
       <c r="A325">
-        <v>1539.97760099341</v>
+        <v>930.1580904533209</v>
       </c>
       <c r="B325">
-        <v>0.05552393436270764</v>
+        <v>0.09246795470271851</v>
       </c>
     </row>
     <row r="326" spans="1:2">
       <c r="A326">
-        <v>1537.49760529341</v>
+        <v>927.6780947533209</v>
       </c>
       <c r="B326">
-        <v>0.05704492829146512</v>
+        <v>0.09488762464167766</v>
       </c>
     </row>
     <row r="327" spans="1:2">
       <c r="A327">
-        <v>1543.08191353341</v>
+        <v>933.262402993321</v>
       </c>
       <c r="B327">
-        <v>0.05362004375261287</v>
+        <v>0.08943915439706818</v>
       </c>
     </row>
     <row r="328" spans="1:2">
       <c r="A328">
-        <v>1549.99779845341</v>
+        <v>940.1782879133209</v>
       </c>
       <c r="B328">
-        <v>0.04937849648892001</v>
+        <v>0.08269149800305742</v>
       </c>
     </row>
     <row r="329" spans="1:2">
       <c r="A329">
-        <v>1547.75930057735</v>
+        <v>937.9397900372609</v>
       </c>
       <c r="B329">
-        <v>0.05075137857860423</v>
+        <v>0.08487554453955992</v>
       </c>
     </row>
     <row r="330" spans="1:2">
       <c r="A330">
-        <v>1545.35048088735</v>
+        <v>935.5309703472609</v>
       </c>
       <c r="B330">
-        <v>0.05222871989978517</v>
+        <v>0.08722576982110608</v>
       </c>
     </row>
     <row r="331" spans="1:2">
       <c r="A331">
-        <v>1540.10128010735</v>
+        <v>930.2817695672609</v>
       </c>
       <c r="B331">
-        <v>0.05544808133545576</v>
+        <v>0.09234728407652448</v>
       </c>
     </row>
     <row r="332" spans="1:2">
       <c r="A332">
-        <v>1538.73430327735</v>
+        <v>928.9147927372609</v>
       </c>
       <c r="B332">
-        <v>0.0562864551516612</v>
+        <v>0.09368100926919498</v>
       </c>
     </row>
     <row r="333" spans="1:2">
       <c r="A333">
-        <v>1538.99104573735</v>
+        <v>929.1715351972609</v>
       </c>
       <c r="B333">
-        <v>0.05612899370004887</v>
+        <v>0.09343051205562469</v>
       </c>
     </row>
     <row r="334" spans="1:2">
       <c r="A334">
-        <v>1535.24658008735</v>
+        <v>925.4270695472609</v>
       </c>
       <c r="B334">
-        <v>0.05842549345611336</v>
+        <v>0.09708389378155668</v>
       </c>
     </row>
     <row r="335" spans="1:2">
       <c r="A335">
-        <v>1534.37041291735</v>
+        <v>924.550902377261</v>
       </c>
       <c r="B335">
-        <v>0.05896285122094591</v>
+        <v>0.09793874823261539</v>
       </c>
     </row>
     <row r="336" spans="1:2">
       <c r="A336">
-        <v>1535.53501914735</v>
+        <v>925.715508607261</v>
       </c>
       <c r="B336">
-        <v>0.05824859231911672</v>
+        <v>0.09680247098606398</v>
       </c>
     </row>
     <row r="337" spans="1:2">
       <c r="A337">
-        <v>1538.21216274735</v>
+        <v>928.3926522072609</v>
       </c>
       <c r="B337">
-        <v>0.05660668658435608</v>
+        <v>0.09419044875909133</v>
       </c>
     </row>
     <row r="338" spans="1:2">
       <c r="A338">
-        <v>1535.79590654735</v>
+        <v>925.976396007261</v>
       </c>
       <c r="B338">
-        <v>0.05808858875480027</v>
+        <v>0.09654792965793457</v>
       </c>
     </row>
     <row r="339" spans="1:2">
       <c r="A339">
-        <v>1534.48488640735</v>
+        <v>924.6653758672609</v>
       </c>
       <c r="B339">
-        <v>0.05889264404950045</v>
+        <v>0.09782705930405777</v>
       </c>
     </row>
     <row r="340" spans="1:2">
       <c r="A340">
-        <v>1536.84494209735</v>
+        <v>927.025431557261</v>
       </c>
       <c r="B340">
-        <v>0.05744520993660296</v>
+        <v>0.09552441184085347</v>
       </c>
     </row>
     <row r="341" spans="1:2">
       <c r="A341">
-        <v>1540.34229617735</v>
+        <v>930.5227856372609</v>
       </c>
       <c r="B341">
-        <v>0.05530026495851481</v>
+        <v>0.09211213070936941</v>
       </c>
     </row>
     <row r="342" spans="1:2">
       <c r="A342">
-        <v>1537.63077395735</v>
+        <v>927.8112634172609</v>
       </c>
       <c r="B342">
-        <v>0.05696325527511525</v>
+        <v>0.09475769529827316</v>
       </c>
     </row>
     <row r="343" spans="1:2">
       <c r="A343">
-        <v>1534.57968694351</v>
+        <v>924.7601764034209</v>
       </c>
       <c r="B343">
-        <v>0.05883450240032662</v>
+        <v>0.09773456478580367</v>
       </c>
     </row>
     <row r="344" spans="1:2">
       <c r="A344">
-        <v>1533.36928534351</v>
+        <v>923.5497748034209</v>
       </c>
       <c r="B344">
-        <v>0.05957684783461836</v>
+        <v>0.09891552343246113</v>
       </c>
     </row>
     <row r="345" spans="1:2">
       <c r="A345">
-        <v>1535.17566774351</v>
+        <v>925.3561572034209</v>
       </c>
       <c r="B345">
-        <v>0.05846898435589765</v>
+        <v>0.09715308118647459</v>
       </c>
     </row>
     <row r="346" spans="1:2">
       <c r="A346">
-        <v>1535.76545270351</v>
+        <v>925.9459421634209</v>
       </c>
       <c r="B346">
-        <v>0.05810726625153473</v>
+        <v>0.0965776427136732</v>
       </c>
     </row>
     <row r="347" spans="1:2">
       <c r="A347">
-        <v>1541.16542230351</v>
+        <v>931.345911763421</v>
       </c>
       <c r="B347">
-        <v>0.05479543753462413</v>
+        <v>0.0913090270816328</v>
       </c>
     </row>
     <row r="348" spans="1:2">
       <c r="A348">
-        <v>1537.61491094351</v>
+        <v>927.7954004034209</v>
       </c>
       <c r="B348">
-        <v>0.05697298414188012</v>
+        <v>0.09477317244516092</v>
       </c>
     </row>
     <row r="349" spans="1:2">
       <c r="A349">
-        <v>1548.68407414351</v>
+        <v>938.8645636034208</v>
       </c>
       <c r="B349">
-        <v>0.05018421026472164</v>
+        <v>0.08397326604029431</v>
       </c>
     </row>
     <row r="350" spans="1:2">
       <c r="A350">
-        <v>1560.54306744921</v>
+        <v>950.7235569091209</v>
       </c>
       <c r="B350">
-        <v>0.04291102958172899</v>
+        <v>0.07240274210425712</v>
       </c>
     </row>
     <row r="351" spans="1:2">
       <c r="A351">
-        <v>1552.33951128921</v>
+        <v>942.520000749121</v>
       </c>
       <c r="B351">
-        <v>0.04794231214144506</v>
+        <v>0.08040674720511853</v>
       </c>
     </row>
     <row r="352" spans="1:2">
       <c r="A352">
-        <v>1556.215654339755</v>
+        <v>946.3961437996653</v>
       </c>
       <c r="B352">
-        <v>0.04556505396842758</v>
+        <v>0.07662489112427651</v>
       </c>
     </row>
     <row r="353" spans="1:3">
       <c r="A353">
-        <v>1559.408170819755</v>
+        <v>949.5886602796652</v>
       </c>
       <c r="B353">
-        <v>0.0436070674350082</v>
+        <v>0.07351003243468801</v>
       </c>
     </row>
     <row r="354" spans="1:3">
       <c r="A354">
-        <v>1556.536321525033</v>
+        <v>946.9184836396653</v>
       </c>
       <c r="B354">
-        <v>0.04536838715890035</v>
+        <v>0.07611525717258505</v>
       </c>
     </row>
     <row r="355" spans="1:3">
       <c r="A355">
-        <v>1555.139063021976</v>
+        <v>944.9144221996653</v>
       </c>
       <c r="B355">
-        <v>0.04622533287862662</v>
+        <v>0.07807056992663342</v>
       </c>
     </row>
     <row r="356" spans="1:3">
       <c r="A356">
-        <v>1555.069728461976</v>
+        <v>944.8100714796652</v>
       </c>
       <c r="B356">
-        <v>0.04626785611558748</v>
+        <v>0.07817238232102297</v>
       </c>
     </row>
     <row r="357" spans="1:3">
       <c r="A357">
-        <v>1550.989744833016</v>
+        <v>939.0983938107053</v>
       </c>
       <c r="B357">
-        <v>0.04877013074819181</v>
+        <v>0.08374512374013354</v>
       </c>
     </row>
     <row r="358" spans="1:3">
       <c r="A358">
-        <v>1551.670125753016</v>
+        <v>940.0540843707053</v>
       </c>
       <c r="B358">
-        <v>0.04835284968251807</v>
+        <v>0.08281268030122801</v>
       </c>
     </row>
     <row r="359" spans="1:3">
       <c r="A359">
-        <v>1563.103393553016</v>
+        <v>956.1137147707053</v>
       </c>
       <c r="B359">
-        <v>0.0413407686092897</v>
+        <v>0.06714369954062704</v>
       </c>
     </row>
     <row r="360" spans="1:3">
       <c r="A360">
-        <v>1564.936824453016</v>
+        <v>958.6890259707052</v>
       </c>
       <c r="B360">
-        <v>0.04021631614846632</v>
+        <v>0.06463103264604164</v>
       </c>
     </row>
     <row r="361" spans="1:3">
       <c r="A361">
-        <v>1560.150700793016</v>
+        <v>951.9662430907053</v>
       </c>
       <c r="B361">
-        <v>0.0431516700400647</v>
+        <v>0.07119028419671336</v>
       </c>
     </row>
     <row r="362" spans="1:3">
       <c r="A362">
-        <v>1556.95869833235</v>
+        <v>947.8710594411558</v>
       </c>
       <c r="B362">
-        <v>0.04510934132282196</v>
+        <v>0.07518585272585698</v>
       </c>
     </row>
     <row r="363" spans="1:3">
       <c r="A363">
-        <v>1537.08994643235</v>
+        <v>923.0294988411557</v>
       </c>
       <c r="B363">
-        <v>0.05729494753652931</v>
+        <v>0.09942314371013172</v>
       </c>
     </row>
     <row r="364" spans="1:3">
       <c r="A364">
-        <v>1511.57795961235</v>
+        <v>891.1322981611559</v>
       </c>
       <c r="B364">
-        <v>0.07294157832050985</v>
+        <v>0.1305444467117217</v>
       </c>
     </row>
     <row r="365" spans="1:3">
       <c r="A365">
-        <v>1527.89310275235</v>
+        <v>911.5308425211558</v>
       </c>
       <c r="B365">
-        <v>0.0629354183651728</v>
+        <v>0.1106420958381235</v>
       </c>
     </row>
     <row r="366" spans="1:3">
       <c r="A366">
-        <v>1522.73280711235</v>
+        <v>905.0790131611558</v>
       </c>
       <c r="B366">
-        <v>0.06610025382800577</v>
+        <v>0.1169369847984896</v>
       </c>
     </row>
     <row r="367" spans="1:3">
       <c r="A367">
-        <v>1522.72959918235</v>
+        <v>905.0750023411557</v>
       </c>
       <c r="B367">
-        <v>0.06610222126772924</v>
+        <v>0.1169408980555104</v>
       </c>
       <c r="C367" s="2">
         <v>228</v>

</xml_diff>